<commit_message>
update validacion fechas modulo Gerencia OK
</commit_message>
<xml_diff>
--- a/uploads/00_Subir_data_Formato Matriz Consultoria_BHA COVID_15_06_2022_100_casos_reports.xlsx
+++ b/uploads/00_Subir_data_Formato Matriz Consultoria_BHA COVID_15_06_2022_100_casos_reports.xlsx
@@ -817,7 +817,7 @@
     <sheetView tabSelected="1" topLeftCell="T1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A226" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="T1" sqref="T1"/>
-      <selection pane="bottomLeft" activeCell="AH228" sqref="AH228"/>
+      <selection pane="bottomLeft" activeCell="AH227" sqref="AH227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21759,9 +21759,7 @@
       <c r="AG227" s="2">
         <v>1</v>
       </c>
-      <c r="AH227" s="17">
-        <v>44053</v>
-      </c>
+      <c r="AH227" s="17"/>
       <c r="AI227" s="2">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
update script distinct repo gerencia
</commit_message>
<xml_diff>
--- a/uploads/00_Subir_data_Formato Matriz Consultoria_BHA COVID_15_06_2022_100_casos_reports.xlsx
+++ b/uploads/00_Subir_data_Formato Matriz Consultoria_BHA COVID_15_06_2022_100_casos_reports.xlsx
@@ -814,7 +814,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI305"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A226" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="T1" sqref="T1"/>
       <selection pane="bottomLeft" activeCell="AH227" sqref="AH227"/>
@@ -21759,7 +21759,9 @@
       <c r="AG227" s="2">
         <v>1</v>
       </c>
-      <c r="AH227" s="17"/>
+      <c r="AH227" s="17">
+        <v>44053</v>
+      </c>
       <c r="AI227" s="2">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
repo gerencia gestantes OK
</commit_message>
<xml_diff>
--- a/uploads/00_Subir_data_Formato Matriz Consultoria_BHA COVID_15_06_2022_100_casos_reports.xlsx
+++ b/uploads/00_Subir_data_Formato Matriz Consultoria_BHA COVID_15_06_2022_100_casos_reports.xlsx
@@ -15,7 +15,7 @@
     <sheet name="3_BD_Gerencia Nacional FINAL" sheetId="7" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'3_BD_Gerencia Nacional FINAL'!$A$1:$AI$77</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'3_BD_Gerencia Nacional FINAL'!$A$1:$AI$305</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -817,7 +817,7 @@
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A226" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="T1" sqref="T1"/>
-      <selection pane="bottomLeft" activeCell="AH227" sqref="AH227"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21648,7 +21648,7 @@
         <v>6</v>
       </c>
       <c r="AA226" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB226" s="2">
         <v>10</v>
@@ -23397,7 +23397,7 @@
         <v>6</v>
       </c>
       <c r="AA245" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB245" s="2">
         <v>10</v>
@@ -25146,7 +25146,7 @@
         <v>6</v>
       </c>
       <c r="AA264" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB264" s="2">
         <v>10</v>
@@ -26895,7 +26895,7 @@
         <v>6</v>
       </c>
       <c r="AA283" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB283" s="2">
         <v>10</v>
@@ -28644,7 +28644,7 @@
         <v>6</v>
       </c>
       <c r="AA302" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB302" s="2">
         <v>10</v>
@@ -28949,7 +28949,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AI77"/>
+  <autoFilter ref="A1:AI305"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
repo gerencia filtro 08
</commit_message>
<xml_diff>
--- a/uploads/00_Subir_data_Formato Matriz Consultoria_BHA COVID_15_06_2022_100_casos_reports.xlsx
+++ b/uploads/00_Subir_data_Formato Matriz Consultoria_BHA COVID_15_06_2022_100_casos_reports.xlsx
@@ -817,7 +817,7 @@
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A226" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="T1" sqref="T1"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="O232" sqref="O232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21618,7 +21618,7 @@
         <v>44798132</v>
       </c>
       <c r="O226" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P226" s="1"/>
       <c r="Q226" s="3">

</xml_diff>